<commit_message>
incorporate changes requested in video & increase image quality & update git ignore
</commit_message>
<xml_diff>
--- a/Filled_GLA_AEB_start_forms.xlsx
+++ b/Filled_GLA_AEB_start_forms.xlsx
@@ -14893,11 +14893,7 @@
       <c r="AJ20" s="651" t="n"/>
       <c r="AK20" s="651" t="n"/>
       <c r="AL20" s="652" t="n"/>
-      <c r="AM20" s="397" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+      <c r="AM20" s="397" t="inlineStr"/>
       <c r="AN20" s="653" t="n"/>
       <c r="AO20" s="3" t="n"/>
     </row>
@@ -15191,11 +15187,7 @@
       <c r="AJ26" s="651" t="n"/>
       <c r="AK26" s="651" t="n"/>
       <c r="AL26" s="652" t="n"/>
-      <c r="AM26" s="397" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+      <c r="AM26" s="397" t="inlineStr"/>
       <c r="AN26" s="653" t="n"/>
       <c r="AO26" s="3" t="n"/>
     </row>
@@ -15408,11 +15400,7 @@
       <c r="F31" s="651" t="n"/>
       <c r="G31" s="651" t="n"/>
       <c r="H31" s="652" t="n"/>
-      <c r="I31" s="747" t="inlineStr">
-        <is>
-          <t>2000-01-01</t>
-        </is>
-      </c>
+      <c r="I31" s="747" t="inlineStr"/>
       <c r="J31" s="657" t="n"/>
       <c r="K31" s="657" t="n"/>
       <c r="L31" s="657" t="n"/>
@@ -15479,11 +15467,7 @@
       <c r="F32" s="651" t="n"/>
       <c r="G32" s="651" t="n"/>
       <c r="H32" s="652" t="n"/>
-      <c r="I32" s="747" t="inlineStr">
-        <is>
-          <t>2000-01-01</t>
-        </is>
-      </c>
+      <c r="I32" s="747" t="inlineStr"/>
       <c r="J32" s="657" t="n"/>
       <c r="K32" s="657" t="n"/>
       <c r="L32" s="657" t="n"/>
@@ -15550,11 +15534,7 @@
       <c r="F33" s="671" t="n"/>
       <c r="G33" s="671" t="n"/>
       <c r="H33" s="670" t="n"/>
-      <c r="I33" s="438" t="inlineStr">
-        <is>
-          <t>Use this space for additional notes where relevant (type of Visa, restrictions, expiry etc.)</t>
-        </is>
-      </c>
+      <c r="I33" s="438" t="inlineStr"/>
       <c r="J33" s="688" t="n"/>
       <c r="K33" s="688" t="n"/>
       <c r="L33" s="688" t="n"/>
@@ -15951,7 +15931,7 @@
       <c r="J40" s="670" t="n"/>
       <c r="K40" s="754" t="inlineStr">
         <is>
-          <t>2000-01-01</t>
+          <t>2024-07-14</t>
         </is>
       </c>
       <c r="L40" s="695" t="n"/>
@@ -16198,7 +16178,7 @@
       <c r="H44" s="670" t="n"/>
       <c r="I44" s="754" t="inlineStr">
         <is>
-          <t>2000-01-01</t>
+          <t>2024-07-14</t>
         </is>
       </c>
       <c r="J44" s="695" t="n"/>
@@ -16333,7 +16313,7 @@
       <c r="AK46" s="644" t="n"/>
       <c r="AL46" s="420" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="AM46" s="683" t="n"/>
@@ -16930,7 +16910,7 @@
       <c r="H58" s="672" t="n"/>
       <c r="I58" s="754" t="inlineStr">
         <is>
-          <t>2000-01-01</t>
+          <t>2024-07-14</t>
         </is>
       </c>
       <c r="J58" s="695" t="n"/>
@@ -17460,7 +17440,7 @@
       <c r="H68" s="652" t="n"/>
       <c r="I68" s="622" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>p65</t>
         </is>
       </c>
       <c r="J68" s="653" t="n"/>
@@ -17478,7 +17458,7 @@
       <c r="R68" s="652" t="n"/>
       <c r="S68" s="622" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>p66</t>
         </is>
       </c>
       <c r="T68" s="653" t="n"/>
@@ -17496,7 +17476,7 @@
       <c r="AB68" s="652" t="n"/>
       <c r="AC68" s="622" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>p67</t>
         </is>
       </c>
       <c r="AD68" s="653" t="n"/>
@@ -17514,7 +17494,7 @@
       <c r="AL68" s="652" t="n"/>
       <c r="AM68" s="767" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>p68</t>
         </is>
       </c>
       <c r="AN68" s="658" t="n"/>
@@ -17535,7 +17515,7 @@
       <c r="H69" s="652" t="n"/>
       <c r="I69" s="622" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>p69</t>
         </is>
       </c>
       <c r="J69" s="653" t="n"/>
@@ -17553,7 +17533,7 @@
       <c r="R69" s="652" t="n"/>
       <c r="S69" s="622" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>p70</t>
         </is>
       </c>
       <c r="T69" s="653" t="n"/>
@@ -17571,7 +17551,7 @@
       <c r="AB69" s="652" t="n"/>
       <c r="AC69" s="622" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>p71</t>
         </is>
       </c>
       <c r="AD69" s="653" t="n"/>
@@ -17589,7 +17569,7 @@
       <c r="AL69" s="652" t="n"/>
       <c r="AM69" s="767" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>p72</t>
         </is>
       </c>
       <c r="AN69" s="658" t="n"/>
@@ -17611,7 +17591,11 @@
       <c r="I70" s="671" t="n"/>
       <c r="J70" s="671" t="n"/>
       <c r="K70" s="670" t="n"/>
-      <c r="L70" s="387" t="inlineStr"/>
+      <c r="L70" s="387" t="inlineStr">
+        <is>
+          <t>p73</t>
+        </is>
+      </c>
       <c r="M70" s="688" t="n"/>
       <c r="N70" s="688" t="n"/>
       <c r="O70" s="688" t="n"/>
@@ -17751,7 +17735,7 @@
       <c r="L73" s="651" t="n"/>
       <c r="M73" s="397" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>p74</t>
         </is>
       </c>
       <c r="N73" s="653" t="n"/>
@@ -17766,7 +17750,7 @@
       <c r="S73" s="652" t="n"/>
       <c r="T73" s="397" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>p75</t>
         </is>
       </c>
       <c r="U73" s="653" t="n"/>
@@ -17781,7 +17765,7 @@
       <c r="Z73" s="652" t="n"/>
       <c r="AA73" s="459" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>p76</t>
         </is>
       </c>
       <c r="AB73" s="653" t="n"/>
@@ -17796,7 +17780,7 @@
       <c r="AG73" s="652" t="n"/>
       <c r="AH73" s="397" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>p77</t>
         </is>
       </c>
       <c r="AI73" s="653" t="n"/>
@@ -17830,7 +17814,7 @@
       <c r="L74" s="651" t="n"/>
       <c r="M74" s="397" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>p78</t>
         </is>
       </c>
       <c r="N74" s="653" t="n"/>
@@ -17845,7 +17829,7 @@
       <c r="S74" s="652" t="n"/>
       <c r="T74" s="397" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>p79</t>
         </is>
       </c>
       <c r="U74" s="653" t="n"/>
@@ -17860,7 +17844,7 @@
       <c r="Z74" s="652" t="n"/>
       <c r="AA74" s="397" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>p80</t>
         </is>
       </c>
       <c r="AB74" s="653" t="n"/>
@@ -17875,7 +17859,7 @@
       <c r="AG74" s="652" t="n"/>
       <c r="AH74" s="459" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>p81</t>
         </is>
       </c>
       <c r="AI74" s="653" t="n"/>
@@ -17909,7 +17893,7 @@
       <c r="L75" s="673" t="n"/>
       <c r="M75" s="626" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>p82</t>
         </is>
       </c>
       <c r="N75" s="696" t="n"/>
@@ -17924,7 +17908,7 @@
       <c r="S75" s="672" t="n"/>
       <c r="T75" s="626" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>p83</t>
         </is>
       </c>
       <c r="U75" s="696" t="n"/>
@@ -17939,7 +17923,7 @@
       <c r="Z75" s="672" t="n"/>
       <c r="AA75" s="626" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>p84</t>
         </is>
       </c>
       <c r="AB75" s="696" t="n"/>
@@ -17954,7 +17938,7 @@
       <c r="AG75" s="672" t="n"/>
       <c r="AH75" s="628" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>p85</t>
         </is>
       </c>
       <c r="AI75" s="696" t="n"/>
@@ -18053,7 +18037,11 @@
       <c r="Z77" s="651" t="n"/>
       <c r="AA77" s="651" t="n"/>
       <c r="AB77" s="652" t="n"/>
-      <c r="AC77" s="397" t="inlineStr"/>
+      <c r="AC77" s="397" t="inlineStr">
+        <is>
+          <t>p86</t>
+        </is>
+      </c>
       <c r="AD77" s="653" t="n"/>
       <c r="AE77" s="406" t="inlineStr">
         <is>
@@ -18067,7 +18055,11 @@
       <c r="AJ77" s="651" t="n"/>
       <c r="AK77" s="651" t="n"/>
       <c r="AL77" s="652" t="n"/>
-      <c r="AM77" s="397" t="inlineStr"/>
+      <c r="AM77" s="397" t="inlineStr">
+        <is>
+          <t>p87</t>
+        </is>
+      </c>
       <c r="AN77" s="653" t="n"/>
       <c r="AO77" s="3" t="n"/>
     </row>
@@ -18108,7 +18100,7 @@
       <c r="AD78" s="652" t="n"/>
       <c r="AE78" s="622" t="inlineStr">
         <is>
-          <t>Y</t>
+          <t>p88</t>
         </is>
       </c>
       <c r="AF78" s="657" t="n"/>
@@ -18116,7 +18108,7 @@
       <c r="AH78" s="653" t="n"/>
       <c r="AI78" s="622" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>p89</t>
         </is>
       </c>
       <c r="AJ78" s="657" t="n"/>
@@ -18163,7 +18155,7 @@
       <c r="AD79" s="652" t="n"/>
       <c r="AE79" s="622" t="inlineStr">
         <is>
-          <t>Y</t>
+          <t>p90</t>
         </is>
       </c>
       <c r="AF79" s="657" t="n"/>
@@ -18171,7 +18163,7 @@
       <c r="AH79" s="653" t="n"/>
       <c r="AI79" s="622" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>p91</t>
         </is>
       </c>
       <c r="AJ79" s="657" t="n"/>
@@ -18197,7 +18189,11 @@
       <c r="I80" s="671" t="n"/>
       <c r="J80" s="671" t="n"/>
       <c r="K80" s="670" t="n"/>
-      <c r="L80" s="387" t="inlineStr"/>
+      <c r="L80" s="387" t="inlineStr">
+        <is>
+          <t>p92</t>
+        </is>
+      </c>
       <c r="M80" s="688" t="n"/>
       <c r="N80" s="688" t="n"/>
       <c r="O80" s="688" t="n"/>
@@ -18387,7 +18383,7 @@
       <c r="O84" s="652" t="n"/>
       <c r="P84" s="760" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q84" s="657" t="n"/>
@@ -19110,7 +19106,11 @@
       <c r="F100" s="671" t="n"/>
       <c r="G100" s="671" t="n"/>
       <c r="H100" s="670" t="n"/>
-      <c r="I100" s="510" t="inlineStr"/>
+      <c r="I100" s="510" t="inlineStr">
+        <is>
+          <t>p103</t>
+        </is>
+      </c>
       <c r="J100" s="688" t="n"/>
       <c r="K100" s="688" t="n"/>
       <c r="L100" s="688" t="n"/>

</xml_diff>